<commit_message>
Add - Fix: Se ordena el código fuente y se aplica el ruido y filtro
Se ordena el código para que solo ejecute la wavelet a utilizar, es decir la Wavelet AMOR. También se crea una función encargada de aplicar el ruido blanco gaussiano y el filtro Butterworth de octavo orden con una frecuencia de corte de 0.25 [Hz]. Posterior a ello se crea una carpeta llamada "signals_noises" donde se almacenan en forma de archivo .csv todas las nuevas señales VSC con ruido y filtro.
</commit_message>
<xml_diff>
--- a/codigo_matlab/Configuración de banco de filtros y comparación del error NMSE.xlsx
+++ b/codigo_matlab/Configuración de banco de filtros y comparación del error NMSE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\codigo_matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B172B3F-00EB-4A4B-97AA-FED6E03ED82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1928829-1A73-40D6-86F6-CA427B1D950E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{546CBC35-C41A-4C5F-9A5B-D35005C1BB7E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{546CBC35-C41A-4C5F-9A5B-D35005C1BB7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Error - banco de filtros" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>G2_001.csv</t>
   </si>
@@ -285,6 +285,45 @@
   <si>
     <t>Análisis: Error calculado en base a la magnitud de los coeficientes reales ()</t>
   </si>
+  <si>
+    <t>ELEGIDA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se bien todas las wavelet presentan un error NMSE bastante bajo, del orden de e-30, se </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>decide por optar AMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> principalmente por el enfoque que le da a las señales, esto es, enfocarse en cambios transitorios y bruscos que se puedan dar en la señal que se está estudiante.  A esta señal se le debe especificar un hiperparámetro denominado VoicesPerOctave, entre menor sea su valor escalar ([1,48]) presenta una mayor resolución temporal pero una menor resolución en el dominio de la frecuencia. </t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -293,7 +332,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,8 +370,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +467,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -459,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -485,33 +553,42 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
@@ -521,26 +598,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,392 +962,467 @@
   </sheetPr>
   <dimension ref="B3:S37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
     </row>
     <row r="14" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="17" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R22" s="28"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+    </row>
+    <row r="27" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="15" t="s">
+      <c r="D27" s="18"/>
+      <c r="E27" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="15" t="s">
+      <c r="F27" s="18"/>
+      <c r="G27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="16"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11">
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24">
         <v>3</v>
       </c>
-      <c r="H28" s="11"/>
+      <c r="H28" s="24"/>
       <c r="I28" s="3">
         <v>1.1674E-30</v>
       </c>
+      <c r="J28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>2</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13">
+      <c r="D29" s="25"/>
+      <c r="E29" s="19">
         <v>10</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="13">
+      <c r="F29" s="20"/>
+      <c r="G29" s="19">
         <v>2</v>
       </c>
-      <c r="H29" s="14"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="5">
         <v>1.0746999999999999E-30</v>
       </c>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" s="7">
         <v>3</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="9">
+      <c r="D30" s="27"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="26">
         <v>6</v>
       </c>
-      <c r="H30" s="10"/>
+      <c r="H30" s="27"/>
       <c r="I30" s="8">
         <v>1.3277E-30</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="29"/>
+      <c r="S31" s="29"/>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
+      <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
+      <c r="S32" s="29"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="15" t="s">
+      <c r="D34" s="18"/>
+      <c r="E34" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="16"/>
-      <c r="G34" s="15" t="s">
+      <c r="F34" s="18"/>
+      <c r="G34" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H34" s="16"/>
+      <c r="H34" s="18"/>
       <c r="I34" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>1</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11">
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24">
         <v>5</v>
       </c>
-      <c r="H35" s="11"/>
+      <c r="H35" s="24"/>
       <c r="I35" s="3">
         <v>1.0246E-30</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>2</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13">
+      <c r="D36" s="25"/>
+      <c r="E36" s="19">
         <v>3</v>
       </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="13">
+      <c r="F36" s="20"/>
+      <c r="G36" s="19">
         <v>4</v>
       </c>
-      <c r="H36" s="14"/>
+      <c r="H36" s="20"/>
       <c r="I36" s="5">
         <v>8.9918E-30</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="7">
         <v>3</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="9">
+      <c r="D37" s="27"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="26">
         <v>7</v>
       </c>
-      <c r="H37" s="10"/>
+      <c r="H37" s="27"/>
       <c r="I37" s="8">
         <v>1.1055000000000001E-30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
+    <mergeCell ref="K28:S32"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="J15:S18"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="G29:H29"/>
@@ -1292,18 +1439,6 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="G35:H35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1317,24 +1452,24 @@
   </sheetPr>
   <dimension ref="B3:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1345,40 +1480,40 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="13">
         <v>0.17510000000000001</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="23">
+      <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="14">
         <v>0.27239999999999998</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="24">
+      <c r="B9" s="12">
         <v>3</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="15">
         <v>0.54139999999999999</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1389,35 +1524,35 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="22">
+      <c r="B13" s="10">
         <v>1</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="13">
         <v>0.7742</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="23">
+      <c r="B14" s="11">
         <v>2</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="14">
         <v>0.8054</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="24">
+      <c r="B15" s="12">
         <v>3</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="15">
         <v>0.87419999999999998</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add - Se termina el bucle que crea estructura única y aplica CWT
Se almacena en la estructura de ruidos, todo lo necesario para trabajar con la red. esto incluye información retornada por la transformada continua Wavelet.
</commit_message>
<xml_diff>
--- a/codigo_matlab/Configuración de banco de filtros y comparación del error NMSE.xlsx
+++ b/codigo_matlab/Configuración de banco de filtros y comparación del error NMSE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\codigo_matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1928829-1A73-40D6-86F6-CA427B1D950E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4FB655-965D-4A1A-B113-3112AE2ED9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{546CBC35-C41A-4C5F-9A5B-D35005C1BB7E}"/>
   </bookViews>
@@ -574,45 +574,45 @@
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -969,382 +969,382 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
     </row>
     <row r="14" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="16" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="26"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="R22" s="28"/>
+      <c r="R22" s="16"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="17" t="s">
+      <c r="D27" s="25"/>
+      <c r="E27" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="17" t="s">
+      <c r="F27" s="25"/>
+      <c r="G27" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="18"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24">
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20">
         <v>3</v>
       </c>
-      <c r="H28" s="24"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="3">
         <v>1.1674E-30</v>
       </c>
       <c r="J28" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="29" t="s">
+      <c r="K28" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="29"/>
-      <c r="R28" s="29"/>
-      <c r="S28" s="29"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>2</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="19">
+      <c r="D29" s="21"/>
+      <c r="E29" s="22">
         <v>10</v>
       </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="19">
+      <c r="F29" s="23"/>
+      <c r="G29" s="22">
         <v>2</v>
       </c>
-      <c r="H29" s="20"/>
+      <c r="H29" s="23"/>
       <c r="I29" s="5">
         <v>1.0746999999999999E-30</v>
       </c>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
-      <c r="O29" s="29"/>
-      <c r="P29" s="29"/>
-      <c r="Q29" s="29"/>
-      <c r="R29" s="29"/>
-      <c r="S29" s="29"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" s="7">
         <v>3</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="26">
+      <c r="D30" s="19"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="18">
         <v>6</v>
       </c>
-      <c r="H30" s="27"/>
+      <c r="H30" s="19"/>
       <c r="I30" s="8">
         <v>1.3277E-30</v>
       </c>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="29"/>
-      <c r="Q30" s="29"/>
-      <c r="R30" s="29"/>
-      <c r="S30" s="29"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="29"/>
-      <c r="Q31" s="29"/>
-      <c r="R31" s="29"/>
-      <c r="S31" s="29"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
-      <c r="R32" s="29"/>
-      <c r="S32" s="29"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="17" t="s">
+      <c r="D34" s="25"/>
+      <c r="E34" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="18"/>
-      <c r="G34" s="17" t="s">
+      <c r="F34" s="25"/>
+      <c r="G34" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H34" s="18"/>
+      <c r="H34" s="25"/>
       <c r="I34" s="6" t="s">
         <v>4</v>
       </c>
@@ -1353,16 +1353,16 @@
       <c r="B35" s="2">
         <v>1</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24">
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20">
         <v>5</v>
       </c>
-      <c r="H35" s="24"/>
+      <c r="H35" s="20"/>
       <c r="I35" s="3">
         <v>1.0246E-30</v>
       </c>
@@ -1374,18 +1374,18 @@
       <c r="B36" s="4">
         <v>2</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="19">
+      <c r="D36" s="21"/>
+      <c r="E36" s="22">
         <v>3</v>
       </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="19">
+      <c r="F36" s="23"/>
+      <c r="G36" s="22">
         <v>4</v>
       </c>
-      <c r="H36" s="20"/>
+      <c r="H36" s="23"/>
       <c r="I36" s="5">
         <v>8.9918E-30</v>
       </c>
@@ -1394,35 +1394,22 @@
       <c r="B37" s="7">
         <v>3</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="27"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="26">
+      <c r="D37" s="19"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="18">
         <v>7</v>
       </c>
-      <c r="H37" s="27"/>
+      <c r="H37" s="19"/>
       <c r="I37" s="8">
         <v>1.1055000000000001E-30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="K28:S32"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="G34:H34"/>
     <mergeCell ref="J15:S18"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="G29:H29"/>
@@ -1439,6 +1426,19 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
+    <mergeCell ref="K28:S32"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="G34:H34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1459,14 +1459,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">

</xml_diff>